<commit_message>
Versão 4 do índice Nupe das empresas cearenses listadas em bolsa.
1 - Inclusão de tabela estatística;
2 - Inclusão de tabela de retornos;
3 - Inclusão de tabela do modelo CAPM;
4 - Download da quantidade de ações em circulação.
</commit_message>
<xml_diff>
--- a/data/exemplo_indices.xlsx
+++ b/data/exemplo_indices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a548da2118d25344/Alysson/Unifor/Monitoria/indice_nupe/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="156" documentId="11_B0B943151F963C08801B179E58DF3CED73F9264A" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AAA9D545-21CE-42AE-95DC-F6444A5450A3}"/>
+  <xr:revisionPtr revIDLastSave="180" documentId="11_B0B943151F963C08801B179E58DF3CED73F9264A" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E9AC4AF0-8985-4834-9B39-0EAC8DD1667D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -89,8 +89,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -129,7 +130,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -143,6 +144,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1118,10 +1120,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C0731DC-99A1-4B2A-B4A6-A8C69BD3D7A3}">
-  <dimension ref="A1:Q14"/>
+  <dimension ref="A1:R14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1129,7 +1131,7 @@
     <col min="17" max="17" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1151,7 +1153,7 @@
       </c>
       <c r="L1" s="6"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="4" t="s">
         <v>12</v>
@@ -1191,7 +1193,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2001</v>
       </c>
@@ -1202,8 +1204,8 @@
         <v>3</v>
       </c>
       <c r="D3">
-        <f>B3*$C$3</f>
-        <v>36</v>
+        <f>B3*$C$4</f>
+        <v>48</v>
       </c>
       <c r="F3">
         <v>5</v>
@@ -1212,8 +1214,8 @@
         <v>7</v>
       </c>
       <c r="H3">
-        <f>F3*$G$3</f>
-        <v>35</v>
+        <f>F3*$G$4</f>
+        <v>45</v>
       </c>
       <c r="K3">
         <v>20</v>
@@ -1222,19 +1224,19 @@
         <v>3</v>
       </c>
       <c r="M3">
-        <f>K3*$L$3</f>
-        <v>60</v>
+        <f>K3*$L$4</f>
+        <v>80</v>
       </c>
       <c r="P3">
         <f>M3+H3+D3</f>
-        <v>131</v>
+        <v>173</v>
       </c>
       <c r="Q3" s="5">
-        <f>P3/$P$3</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+        <f>P3/$P$4</f>
+        <v>0.69199999999999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2002</v>
       </c>
@@ -1245,8 +1247,8 @@
         <v>4</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D7" si="0">B4*$C$3</f>
-        <v>45</v>
+        <f t="shared" ref="D4:D7" si="0">B4*$C$4</f>
+        <v>60</v>
       </c>
       <c r="F4">
         <v>10</v>
@@ -1255,8 +1257,8 @@
         <v>9</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H7" si="1">F4*$G$3</f>
-        <v>70</v>
+        <f t="shared" ref="H4:H7" si="1">F4*$G$4</f>
+        <v>90</v>
       </c>
       <c r="K4">
         <v>25</v>
@@ -1265,19 +1267,19 @@
         <v>4</v>
       </c>
       <c r="M4">
-        <f t="shared" ref="M4:M7" si="2">K4*$L$3</f>
-        <v>75</v>
+        <f t="shared" ref="M4:M7" si="2">K4*$L$4</f>
+        <v>100</v>
       </c>
       <c r="P4">
         <f>M4+H4+D4</f>
-        <v>190</v>
+        <v>250</v>
       </c>
       <c r="Q4" s="5">
-        <f t="shared" ref="Q4:Q7" si="3">P4/$P$3</f>
-        <v>1.4503816793893129</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+        <f>P4/$P$4</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2003</v>
       </c>
@@ -1289,7 +1291,7 @@
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="F5">
         <v>20</v>
@@ -1299,7 +1301,7 @@
       </c>
       <c r="H5">
         <f t="shared" si="1"/>
-        <v>140</v>
+        <v>180</v>
       </c>
       <c r="K5">
         <v>35</v>
@@ -1309,18 +1311,22 @@
       </c>
       <c r="M5">
         <f t="shared" si="2"/>
-        <v>105</v>
+        <v>140</v>
       </c>
       <c r="P5">
         <f>M5+H5+D5</f>
-        <v>299</v>
+        <v>392</v>
       </c>
       <c r="Q5" s="5">
-        <f t="shared" si="3"/>
-        <v>2.282442748091603</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+        <f t="shared" ref="Q5:Q7" si="3">P5/$P$4</f>
+        <v>1.5680000000000001</v>
+      </c>
+      <c r="R5">
+        <f>Q5/Q4</f>
+        <v>1.5680000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2004</v>
       </c>
@@ -1332,7 +1338,7 @@
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="F6">
         <v>30</v>
@@ -1342,7 +1348,7 @@
       </c>
       <c r="H6">
         <f t="shared" si="1"/>
-        <v>210</v>
+        <v>270</v>
       </c>
       <c r="K6">
         <v>45</v>
@@ -1352,18 +1358,22 @@
       </c>
       <c r="M6">
         <f t="shared" si="2"/>
-        <v>135</v>
+        <v>180</v>
       </c>
       <c r="P6">
         <f>M6+H6+D6</f>
-        <v>417</v>
+        <v>546</v>
       </c>
       <c r="Q6" s="5">
         <f t="shared" si="3"/>
-        <v>3.1832061068702289</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+        <v>2.1840000000000002</v>
+      </c>
+      <c r="R6">
+        <f t="shared" ref="R6:R7" si="4">Q6/Q5</f>
+        <v>1.392857142857143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2005</v>
       </c>
@@ -1375,7 +1385,7 @@
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="F7">
         <v>60</v>
@@ -1385,7 +1395,7 @@
       </c>
       <c r="H7">
         <f t="shared" si="1"/>
-        <v>420</v>
+        <v>540</v>
       </c>
       <c r="K7">
         <v>50</v>
@@ -1395,18 +1405,29 @@
       </c>
       <c r="M7">
         <f t="shared" si="2"/>
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="P7">
         <f>M7+H7+D7</f>
-        <v>660</v>
+        <v>860</v>
       </c>
       <c r="Q7" s="5">
         <f t="shared" si="3"/>
-        <v>5.0381679389312977</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+        <v>3.44</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="4"/>
+        <v>1.575091575091575</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q9" s="5"/>
+      <c r="R9" s="7">
+        <f>PRODUCT(R5:R7)</f>
+        <v>3.44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2001</v>
       </c>
@@ -1427,87 +1448,87 @@
         <v>131</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2002</v>
       </c>
       <c r="B11">
-        <f t="shared" ref="B11:B14" si="4">B4*C4</f>
+        <f t="shared" ref="B11:B14" si="5">B4*C4</f>
         <v>60</v>
       </c>
       <c r="C11">
-        <f t="shared" ref="C11:C14" si="5">F4*G4</f>
+        <f t="shared" ref="C11:C14" si="6">F4*G4</f>
         <v>90</v>
       </c>
       <c r="D11">
-        <f t="shared" ref="D11:D14" si="6">K4*L4</f>
+        <f t="shared" ref="D11:D14" si="7">K4*L4</f>
         <v>100</v>
       </c>
       <c r="E11">
-        <f t="shared" ref="E11:E14" si="7">SUM(B11:D11)</f>
+        <f t="shared" ref="E11:E14" si="8">SUM(B11:D11)</f>
         <v>250</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2003</v>
       </c>
       <c r="B12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>90</v>
       </c>
       <c r="C12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>160</v>
       </c>
       <c r="D12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>175</v>
       </c>
       <c r="E12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>425</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2004</v>
       </c>
       <c r="B13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>120</v>
       </c>
       <c r="C13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>210</v>
       </c>
       <c r="D13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>270</v>
       </c>
       <c r="E13">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>600</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2005</v>
       </c>
       <c r="B14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>180</v>
       </c>
       <c r="C14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>360</v>
       </c>
       <c r="D14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>250</v>
       </c>
       <c r="E14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>790</v>
       </c>
     </row>

</xml_diff>